<commit_message>
evidence update & refactor
</commit_message>
<xml_diff>
--- a/delta2/lib_e/linuxlol.xlsx
+++ b/delta2/lib_e/linuxlol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harveywargo/Desktop/GithubProjects/h2w-delta/delta2/lib_e/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B1CE0D-94F6-FA44-ADA8-11336C65AEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A22979D-E613-B345-B357-8AC741A4D524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{2B361B8B-B20C-1B4A-9CA2-9DEA1E5C6017}"/>
+    <workbookView xWindow="80" yWindow="-20840" windowWidth="34560" windowHeight="21100" xr2:uid="{2B361B8B-B20C-1B4A-9CA2-9DEA1E5C6017}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="88">
   <si>
     <t>eid</t>
   </si>
@@ -237,6 +237,71 @@
   </si>
   <si>
     <t>linuxlol-eid0027</t>
+  </si>
+  <si>
+    <t>~/dirtycow$ gcc -pthread c0w.c -o cow</t>
+  </si>
+  <si>
+    <t>~/tools/dirtycow$</t>
+  </si>
+  <si>
+    <t>~/tools/linpeas</t>
+  </si>
+  <si>
+    <t>~/tools/linux-exploit-suggestor</t>
+  </si>
+  <si>
+    <t>~/tools/linenum</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0028</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0029</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0030</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0031</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0032</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0033</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>cat .bash_history</t>
+  </si>
+  <si>
+    <t>grep --color=auto -rnw '/' -ie "PASSWORD" --color=always 2&gt; /dev/null
+find . -type f -exec grep -i -I "PASSWORD" {} /dev/null \;</t>
+  </si>
+  <si>
+    <t>~/tools/linpeas$ ./linpeas.sh</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0034</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0035</t>
+  </si>
+  <si>
+    <t>history | grep pass</t>
+  </si>
+  <si>
+    <t>linuxlol-eid0036</t>
+  </si>
+  <si>
+    <t>find / -name authorized_keys 2&gt; /dev/null
+find / -name id_rsa 2&gt; /dev/null</t>
+  </si>
+  <si>
+    <t>ssh-keygen</t>
   </si>
 </sst>
 </file>
@@ -326,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}" name="Table1" displayName="Table1" ref="A1:G28" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G28" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}" name="Table1" displayName="Table1" ref="A1:G39" totalsRowShown="0" dataDxfId="7">
+  <autoFilter ref="A1:G39" xr:uid="{C77889FB-1522-0A4D-8EB6-D259755FECDF}"/>
   <tableColumns count="7">
     <tableColumn id="7" xr3:uid="{5516EDED-B058-144E-976C-0B23FABA65AE}" name="eid" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{0B947D48-DA4A-7C49-9C7F-01EFE6AFBBF9}" name="map_pid" dataDxfId="5"/>
@@ -658,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADA5849-2682-F643-8842-EFF560F6FB5C}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +736,7 @@
     <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="75" customWidth="1"/>
     <col min="6" max="6" width="31.83203125" customWidth="1"/>
-    <col min="7" max="7" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="53.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -1153,6 +1218,157 @@
         <v>39</v>
       </c>
       <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>